<commit_message>
[MS-OXCPERM]: Fix watchman issues.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCPERM/MS-OXCPERM_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCPERM/MS-OXCPERM_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="508">
   <si>
     <t>Req ID</t>
   </si>
@@ -1733,9 +1733,6 @@
     <t>MS-OXCPERM_R115002</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-OXCPERM_R115001, MS-OXCPERM_R115002.</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] When flag FolderOwner is set, the Implementation does not allow the specified user's client to modify properties. &lt;3&gt; Section 2.2.7:  Exchange 2007 does not allow the properties of a folder to be modified when the FolderOwner flag is set.</t>
   </si>
   <si>
@@ -1770,12 +1767,15 @@
   </si>
   <si>
     <t>[In Appendix A: Product Behavior] &lt;5&gt; Section 2.2.7: Exchange 2007, Exchange 2010, Exchange 2013, and Exchange 2016 include the FreeBusySimple flag by default on the Calendar folder for any entry in the permissions list except the anonymous user and add the FreeBusyDetailed flag to any entries that have the ReadAny flag set. Exchange 2007, Exchange 2010, Exchange 2013, and Exchange 2016 use these defaults until the client modifies the permissions list with the IncludeFreeBusy flag set in the RopModifyPermissions ROP request to override the default value.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXCPERM_R115002.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -2041,6 +2041,21 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2064,21 +2079,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2716,7 +2716,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2749,9 +2749,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2784,6 +2801,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3016,127 +3050,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -3149,12 +3183,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -3167,12 +3201,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -3185,12 +3219,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -3203,60 +3237,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -6196,7 +6230,7 @@
       </c>
       <c r="I135" s="31"/>
     </row>
-    <row r="136" spans="1:9" ht="60">
+    <row r="136" spans="1:9" ht="45">
       <c r="A136" s="29" t="s">
         <v>159</v>
       </c>
@@ -6219,8 +6253,8 @@
       <c r="H136" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I136" s="31" t="s">
-        <v>495</v>
+      <c r="I136" s="20" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="60">
@@ -6247,7 +6281,7 @@
         <v>17</v>
       </c>
       <c r="I137" s="31" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -6532,8 +6566,8 @@
       <c r="B149" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="C149" s="31" t="s">
-        <v>504</v>
+      <c r="C149" s="20" t="s">
+        <v>503</v>
       </c>
       <c r="D149" s="29"/>
       <c r="E149" s="29" t="s">
@@ -7133,7 +7167,7 @@
         <v>33</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="29" t="s">
@@ -8026,14 +8060,14 @@
       <c r="I208" s="31"/>
     </row>
     <row r="209" spans="1:9" ht="45">
-      <c r="A209" s="29" t="s">
+      <c r="A209" s="22" t="s">
         <v>493</v>
       </c>
       <c r="B209" s="30" t="s">
         <v>272</v>
       </c>
       <c r="C209" s="31" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D209" s="29" t="s">
         <v>492</v>
@@ -8048,11 +8082,9 @@
         <v>15</v>
       </c>
       <c r="H209" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I209" s="31" t="s">
-        <v>482</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I209" s="31"/>
     </row>
     <row r="210" spans="1:9" ht="45">
       <c r="A210" s="29" t="s">
@@ -8062,7 +8094,7 @@
         <v>272</v>
       </c>
       <c r="C210" s="31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D210" s="29" t="s">
         <v>492</v>
@@ -8085,16 +8117,16 @@
     </row>
     <row r="211" spans="1:9" ht="45">
       <c r="A211" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B211" s="30" t="s">
         <v>272</v>
       </c>
       <c r="C211" s="31" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E211" s="29" t="s">
         <v>22</v>
@@ -8114,16 +8146,16 @@
     </row>
     <row r="212" spans="1:9" ht="60">
       <c r="A212" s="29" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B212" s="30" t="s">
         <v>272</v>
       </c>
       <c r="C212" s="31" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E212" s="29" t="s">
         <v>22</v>
@@ -8149,7 +8181,7 @@
         <v>272</v>
       </c>
       <c r="C213" s="31" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D213" s="29"/>
       <c r="E213" s="29" t="s">
@@ -8174,7 +8206,7 @@
         <v>272</v>
       </c>
       <c r="C214" s="31" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D214" s="29"/>
       <c r="E214" s="29" t="s">
@@ -8628,11 +8660,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -8640,6 +8667,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H231 A34:I231">
@@ -8728,21 +8760,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -8791,10 +8808,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8814,16 +8853,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-OXCPERM] Update RS according to v20180724
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCPERM/MS-OXCPERM_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCPERM/MS-OXCPERM_RequirementSpecification.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31501B5D-CCCB-4356-A7B1-99E2D3DF12D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -20,8 +21,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmpBC7E" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmpBC7E" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-gufu\AppData\Local\Temp\tmpBC7E.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -1293,9 +1294,6 @@
     <t>[In PidTagAccessControlListData Property] Type: PtypBinary ([MS-OXCDATA] section 2.11.1)</t>
   </si>
   <si>
-    <t>[In PidTagAccessControlListData Property] The PidTagAccessControlListData property ([MS-OXPROPS] section 2.497) contains a variable-length binary large object (BLOB) that constitutes a permissions list for a folder.</t>
-  </si>
-  <si>
     <t>[In PidTagAccessControlListData Property] This property is used when an ACL is copied from one folder to another.&lt;2&gt;</t>
   </si>
   <si>
@@ -1308,9 +1306,6 @@
     <t>[In PidTagEntryId Property] Type: PtypBinary ([MS-OXCDATA] section 2.11.1)</t>
   </si>
   <si>
-    <t>[In PidTagEntryId Property] The PidTagEntryId property ([MS-OXPROPS] section 2.674) identifies the Address Book object that specifies a user.</t>
-  </si>
-  <si>
     <t>[In PidTagEntryId Property] The first two bytes of this property specify the number of bytes that follow.</t>
   </si>
   <si>
@@ -1627,9 +1622,6 @@
   </si>
   <si>
     <t>[In Appendix A: Product Behavior] &lt;1&gt; Section 2.2.2.1: Office Outlook 2003 and Office Outlook 2007 do not set the ReplaceRows flag in the RopModifyPermissions ROP request buffer ([MS-OXCROPS] section 2.2.10.1.1).</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] &lt;2&gt; Section 2.2.3: Outlook 2010 and Outlook 2013 do not use the PidTagAccessControlListData property (section 2.2.3).</t>
   </si>
   <si>
     <t>[In Appendix A: Product Behavior] Implementation does support this specification [MS-OXCMAPIHTTP]. (Exchange Server 2013 Service Pack 1 (SP1) follows this behavior.)</t>
@@ -1703,21 +1695,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>[In PidTagEntryId Property] [The first two bytes of this property specify the number of bytes that follow.] The remaining bytes constitute the PermanentEntryID structure ([MS-OXNSPI] section 2.3.9.3).</t>
   </si>
   <si>
-    <t>[In PidTagMemberId Property] The PidTagMemberId property ([MS-OXPROPS] section 2.773) specifies the unique identifier that the server generates for each user.</t>
-  </si>
-  <si>
-    <t>[In PidTagMemberName Property] The PidTagMemberName property ([MS-OXPROPS] section 2.774) specifies the user-readable name of the user.</t>
-  </si>
-  <si>
-    <t>[In PidTagMemberRights Property] The PidTagMemberRights property ([MS-OXPROPS] section 2.775) specifies the folder permissions that are granted to the specified user.</t>
-  </si>
-  <si>
     <t>[In PidTagMemberRights Property] If this flag [FolderOwner] is not set, the server SHOULD NOT &lt;4&gt; allow the specified user's client to make those modifications [Modifying the folder's properties].</t>
   </si>
   <si>
@@ -1766,16 +1746,37 @@
     <t>[In Appendix A: Product Behavior] &lt;6&gt; Section 3.1.4.2: Office Outlook 2003 and Office Outlook 2007 do not set the ReplaceRows flag in the RopModifyPermissions ROP request buffer ([MS-OXCROPS] section 2.2.10.1.1).</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] &lt;5&gt; Section 2.2.7: Exchange 2007, Exchange 2010, Exchange 2013, and Exchange 2016 include the FreeBusySimple flag by default on the Calendar folder for any entry in the permissions list except the anonymous user and add the FreeBusyDetailed flag to any entries that have the ReadAny flag set. Exchange 2007, Exchange 2010, Exchange 2013, and Exchange 2016 use these defaults until the client modifies the permissions list with the IncludeFreeBusy flag set in the RopModifyPermissions ROP request to override the default value.</t>
-  </si>
-  <si>
     <t>Verified by derived requirement: MS-OXCPERM_R115002.</t>
+  </si>
+  <si>
+    <t>[In PidTagAccessControlListData Property] The PidTagAccessControlListData property ([MS-OXPROPS] section 2.500) contains a variable-length binary large object (BLOB) that constitutes a permissions list for a folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagEntryId Property] The PidTagEntryId property ([MS-OXPROPS] section 2.677) identifies the Address Book object that specifies a user.</t>
+  </si>
+  <si>
+    <t>[In PidTagMemberId Property] The PidTagMemberId property ([MS-OXPROPS] section 2.776) specifies the unique identifier that the server generates for each user.</t>
+  </si>
+  <si>
+    <t>[In PidTagMemberName Property] The PidTagMemberName property ([MS-OXPROPS] section 2.777) specifies the user-readable name of the user.</t>
+  </si>
+  <si>
+    <t>[In PidTagMemberRights Property] The PidTagMemberRights property ([MS-OXPROPS] section 2.778) specifies the folder permissions that are granted to the specified user.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] &lt;2&gt; Section 2.2.3: Outlook 2010, Outlook 2013, Outlook 2016, Outlook 2019 Preview  do not use the PidTagAccessControlListData property (section 2.2.3).</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] &lt;5&gt; Section 2.2.7: Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview include the FreeBusySimple flag by default on the Calendar folder for any entry in the permissions list except the anonymous user and add the FreeBusyDetailed flag to any entries that have the ReadAny flag set. Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview use these defaults until the client modifies the permissions list with the IncludeFreeBusy flag set in the RopModifyPermissions ROP request to override the default value.</t>
+  </si>
+  <si>
+    <t>12.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -2041,21 +2042,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2079,6 +2065,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2626,34 +2627,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I231" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Normal" dataCellStyle="Normal" connectionId="1">
-  <autoFilter ref="A19:I231"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I231" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Normal" dataCellStyle="Normal" connectionId="1">
+  <autoFilter ref="A19:I231" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16" dataCellStyle="Normal">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15" dataCellStyle="Normal">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14" dataCellStyle="Normal">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13" dataCellStyle="Normal">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12" dataCellStyle="Normal">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11" dataCellStyle="Normal">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10" dataCellStyle="Normal">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9" dataCellStyle="Normal">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9" dataCellStyle="Normal">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -2662,12 +2663,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2993,7 +2994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L233"/>
   <sheetViews>
@@ -3015,7 +3016,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -3025,7 +3026,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3039,138 +3040,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>485</v>
+        <v>507</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="12">
-        <v>42535</v>
+        <v>43305</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -3183,12 +3184,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -3201,12 +3202,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -3219,12 +3220,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -3237,60 +3238,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -3573,7 +3574,7 @@
         <v>17</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="23" customFormat="1" ht="30">
@@ -3900,7 +3901,7 @@
         <v>17</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30">
@@ -4002,7 +4003,7 @@
         <v>17</v>
       </c>
       <c r="I46" s="31" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="30">
@@ -5037,8 +5038,8 @@
       <c r="B88" s="30" t="s">
         <v>260</v>
       </c>
-      <c r="C88" s="31" t="s">
-        <v>349</v>
+      <c r="C88" s="20" t="s">
+        <v>500</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="29" t="s">
@@ -5063,7 +5064,7 @@
         <v>260</v>
       </c>
       <c r="C89" s="31" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="29" t="s">
@@ -5088,7 +5089,7 @@
         <v>260</v>
       </c>
       <c r="C90" s="31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="29" t="s">
@@ -5113,7 +5114,7 @@
         <v>260</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="29" t="s">
@@ -5138,7 +5139,7 @@
         <v>261</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D92" s="29"/>
       <c r="E92" s="29" t="s">
@@ -5162,8 +5163,8 @@
       <c r="B93" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="C93" s="31" t="s">
-        <v>354</v>
+      <c r="C93" s="20" t="s">
+        <v>501</v>
       </c>
       <c r="D93" s="29"/>
       <c r="E93" s="29" t="s">
@@ -5188,7 +5189,7 @@
         <v>261</v>
       </c>
       <c r="C94" s="31" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D94" s="29"/>
       <c r="E94" s="29" t="s">
@@ -5213,7 +5214,7 @@
         <v>261</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="D95" s="29"/>
       <c r="E95" s="29" t="s">
@@ -5238,7 +5239,7 @@
         <v>261</v>
       </c>
       <c r="C96" s="31" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D96" s="29"/>
       <c r="E96" s="29" t="s">
@@ -5263,7 +5264,7 @@
         <v>262</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D97" s="29"/>
       <c r="E97" s="29" t="s">
@@ -5287,8 +5288,8 @@
       <c r="B98" s="30" t="s">
         <v>262</v>
       </c>
-      <c r="C98" s="31" t="s">
-        <v>487</v>
+      <c r="C98" s="20" t="s">
+        <v>502</v>
       </c>
       <c r="D98" s="29"/>
       <c r="E98" s="29" t="s">
@@ -5313,7 +5314,7 @@
         <v>262</v>
       </c>
       <c r="C99" s="31" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D99" s="29"/>
       <c r="E99" s="29" t="s">
@@ -5338,7 +5339,7 @@
         <v>262</v>
       </c>
       <c r="C100" s="31" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D100" s="29"/>
       <c r="E100" s="29" t="s">
@@ -5363,7 +5364,7 @@
         <v>262</v>
       </c>
       <c r="C101" s="31" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D101" s="29"/>
       <c r="E101" s="29" t="s">
@@ -5388,7 +5389,7 @@
         <v>263</v>
       </c>
       <c r="C102" s="31" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D102" s="29"/>
       <c r="E102" s="29" t="s">
@@ -5412,8 +5413,8 @@
       <c r="B103" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="C103" s="31" t="s">
-        <v>488</v>
+      <c r="C103" s="20" t="s">
+        <v>503</v>
       </c>
       <c r="D103" s="29"/>
       <c r="E103" s="29" t="s">
@@ -5438,7 +5439,7 @@
         <v>263</v>
       </c>
       <c r="C104" s="31" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D104" s="29"/>
       <c r="E104" s="29" t="s">
@@ -5463,7 +5464,7 @@
         <v>263</v>
       </c>
       <c r="C105" s="31" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D105" s="29"/>
       <c r="E105" s="29" t="s">
@@ -5488,7 +5489,7 @@
         <v>263</v>
       </c>
       <c r="C106" s="31" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D106" s="29"/>
       <c r="E106" s="29" t="s">
@@ -5513,7 +5514,7 @@
         <v>263</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="29" t="s">
@@ -5538,7 +5539,7 @@
         <v>264</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D108" s="29"/>
       <c r="E108" s="29" t="s">
@@ -5562,8 +5563,8 @@
       <c r="B109" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="C109" s="31" t="s">
-        <v>489</v>
+      <c r="C109" s="20" t="s">
+        <v>504</v>
       </c>
       <c r="D109" s="29"/>
       <c r="E109" s="29" t="s">
@@ -5588,7 +5589,7 @@
         <v>264</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D110" s="29"/>
       <c r="E110" s="29" t="s">
@@ -5613,7 +5614,7 @@
         <v>264</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D111" s="29"/>
       <c r="E111" s="29" t="s">
@@ -5638,7 +5639,7 @@
         <v>264</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="29" t="s">
@@ -5663,7 +5664,7 @@
         <v>264</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D113" s="29"/>
       <c r="E113" s="29" t="s">
@@ -5688,7 +5689,7 @@
         <v>264</v>
       </c>
       <c r="C114" s="31" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="29" t="s">
@@ -5713,7 +5714,7 @@
         <v>264</v>
       </c>
       <c r="C115" s="31" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -5738,7 +5739,7 @@
         <v>264</v>
       </c>
       <c r="C116" s="31" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="29" t="s">
@@ -5763,7 +5764,7 @@
         <v>264</v>
       </c>
       <c r="C117" s="31" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="29" t="s">
@@ -5788,7 +5789,7 @@
         <v>264</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="29" t="s">
@@ -5813,7 +5814,7 @@
         <v>264</v>
       </c>
       <c r="C119" s="31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="29" t="s">
@@ -5838,7 +5839,7 @@
         <v>264</v>
       </c>
       <c r="C120" s="31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D120" s="29"/>
       <c r="E120" s="29" t="s">
@@ -5863,7 +5864,7 @@
         <v>264</v>
       </c>
       <c r="C121" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="29" t="s">
@@ -5888,7 +5889,7 @@
         <v>264</v>
       </c>
       <c r="C122" s="31" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="29" t="s">
@@ -5913,7 +5914,7 @@
         <v>264</v>
       </c>
       <c r="C123" s="31" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29" t="s">
@@ -5938,7 +5939,7 @@
         <v>264</v>
       </c>
       <c r="C124" s="31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D124" s="29"/>
       <c r="E124" s="29" t="s">
@@ -5963,7 +5964,7 @@
         <v>264</v>
       </c>
       <c r="C125" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="29" t="s">
@@ -5988,7 +5989,7 @@
         <v>264</v>
       </c>
       <c r="C126" s="31" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="29" t="s">
@@ -6013,7 +6014,7 @@
         <v>264</v>
       </c>
       <c r="C127" s="31" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="29" t="s">
@@ -6038,7 +6039,7 @@
         <v>264</v>
       </c>
       <c r="C128" s="31" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="29" t="s">
@@ -6063,7 +6064,7 @@
         <v>264</v>
       </c>
       <c r="C129" s="31" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="29" t="s">
@@ -6088,7 +6089,7 @@
         <v>264</v>
       </c>
       <c r="C130" s="31" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="29" t="s">
@@ -6113,7 +6114,7 @@
         <v>264</v>
       </c>
       <c r="C131" s="31" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -6138,7 +6139,7 @@
         <v>264</v>
       </c>
       <c r="C132" s="31" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="29" t="s">
@@ -6163,7 +6164,7 @@
         <v>264</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D133" s="29"/>
       <c r="E133" s="29" t="s">
@@ -6188,7 +6189,7 @@
         <v>264</v>
       </c>
       <c r="C134" s="31" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="29" t="s">
@@ -6213,7 +6214,7 @@
         <v>264</v>
       </c>
       <c r="C135" s="31" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="29" t="s">
@@ -6238,7 +6239,7 @@
         <v>264</v>
       </c>
       <c r="C136" s="31" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="29" t="s">
@@ -6254,7 +6255,7 @@
         <v>17</v>
       </c>
       <c r="I136" s="20" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="60">
@@ -6265,7 +6266,7 @@
         <v>264</v>
       </c>
       <c r="C137" s="31" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="29" t="s">
@@ -6281,7 +6282,7 @@
         <v>17</v>
       </c>
       <c r="I137" s="31" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -6292,7 +6293,7 @@
         <v>264</v>
       </c>
       <c r="C138" s="31" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="29" t="s">
@@ -6317,7 +6318,7 @@
         <v>264</v>
       </c>
       <c r="C139" s="31" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="29" t="s">
@@ -6342,7 +6343,7 @@
         <v>264</v>
       </c>
       <c r="C140" s="31" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="29" t="s">
@@ -6367,7 +6368,7 @@
         <v>264</v>
       </c>
       <c r="C141" s="31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="29" t="s">
@@ -6392,7 +6393,7 @@
         <v>264</v>
       </c>
       <c r="C142" s="31" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D142" s="29"/>
       <c r="E142" s="29" t="s">
@@ -6417,7 +6418,7 @@
         <v>264</v>
       </c>
       <c r="C143" s="31" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -6442,7 +6443,7 @@
         <v>264</v>
       </c>
       <c r="C144" s="31" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="29" t="s">
@@ -6467,7 +6468,7 @@
         <v>264</v>
       </c>
       <c r="C145" s="31" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D145" s="29"/>
       <c r="E145" s="29" t="s">
@@ -6492,7 +6493,7 @@
         <v>264</v>
       </c>
       <c r="C146" s="31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D146" s="29"/>
       <c r="E146" s="29" t="s">
@@ -6517,7 +6518,7 @@
         <v>264</v>
       </c>
       <c r="C147" s="31" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D147" s="29"/>
       <c r="E147" s="29" t="s">
@@ -6542,7 +6543,7 @@
         <v>264</v>
       </c>
       <c r="C148" s="31" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D148" s="29"/>
       <c r="E148" s="29" t="s">
@@ -6567,7 +6568,7 @@
         <v>264</v>
       </c>
       <c r="C149" s="20" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="D149" s="29"/>
       <c r="E149" s="29" t="s">
@@ -6592,7 +6593,7 @@
         <v>264</v>
       </c>
       <c r="C150" s="31" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="29" t="s">
@@ -6617,7 +6618,7 @@
         <v>264</v>
       </c>
       <c r="C151" s="31" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D151" s="29"/>
       <c r="E151" s="29" t="s">
@@ -6642,7 +6643,7 @@
         <v>264</v>
       </c>
       <c r="C152" s="31" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="29" t="s">
@@ -6667,7 +6668,7 @@
         <v>264</v>
       </c>
       <c r="C153" s="31" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="29" t="s">
@@ -6692,7 +6693,7 @@
         <v>265</v>
       </c>
       <c r="C154" s="31" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="29" t="s">
@@ -6717,7 +6718,7 @@
         <v>265</v>
       </c>
       <c r="C155" s="31" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="29" t="s">
@@ -6742,7 +6743,7 @@
         <v>265</v>
       </c>
       <c r="C156" s="31" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="29" t="s">
@@ -6767,7 +6768,7 @@
         <v>265</v>
       </c>
       <c r="C157" s="31" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D157" s="29"/>
       <c r="E157" s="29" t="s">
@@ -6792,7 +6793,7 @@
         <v>32</v>
       </c>
       <c r="C158" s="31" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D158" s="29"/>
       <c r="E158" s="29" t="s">
@@ -6817,7 +6818,7 @@
         <v>32</v>
       </c>
       <c r="C159" s="31" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D159" s="29"/>
       <c r="E159" s="29" t="s">
@@ -6842,7 +6843,7 @@
         <v>32</v>
       </c>
       <c r="C160" s="31" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D160" s="29"/>
       <c r="E160" s="29" t="s">
@@ -6867,7 +6868,7 @@
         <v>32</v>
       </c>
       <c r="C161" s="31" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D161" s="29"/>
       <c r="E161" s="29" t="s">
@@ -6892,7 +6893,7 @@
         <v>32</v>
       </c>
       <c r="C162" s="31" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D162" s="29"/>
       <c r="E162" s="29" t="s">
@@ -6917,7 +6918,7 @@
         <v>32</v>
       </c>
       <c r="C163" s="31" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D163" s="29"/>
       <c r="E163" s="29" t="s">
@@ -6942,7 +6943,7 @@
         <v>32</v>
       </c>
       <c r="C164" s="31" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D164" s="29"/>
       <c r="E164" s="29" t="s">
@@ -6967,7 +6968,7 @@
         <v>32</v>
       </c>
       <c r="C165" s="31" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="29" t="s">
@@ -6992,7 +6993,7 @@
         <v>32</v>
       </c>
       <c r="C166" s="31" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D166" s="29"/>
       <c r="E166" s="29" t="s">
@@ -7017,7 +7018,7 @@
         <v>32</v>
       </c>
       <c r="C167" s="31" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D167" s="29"/>
       <c r="E167" s="29" t="s">
@@ -7042,7 +7043,7 @@
         <v>32</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D168" s="29"/>
       <c r="E168" s="29" t="s">
@@ -7067,7 +7068,7 @@
         <v>32</v>
       </c>
       <c r="C169" s="31" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D169" s="29"/>
       <c r="E169" s="29" t="s">
@@ -7092,7 +7093,7 @@
         <v>33</v>
       </c>
       <c r="C170" s="31" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D170" s="29"/>
       <c r="E170" s="29" t="s">
@@ -7117,7 +7118,7 @@
         <v>33</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D171" s="29"/>
       <c r="E171" s="29" t="s">
@@ -7142,7 +7143,7 @@
         <v>33</v>
       </c>
       <c r="C172" s="31" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D172" s="29"/>
       <c r="E172" s="29" t="s">
@@ -7167,7 +7168,7 @@
         <v>33</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="29" t="s">
@@ -7192,7 +7193,7 @@
         <v>33</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D174" s="29"/>
       <c r="E174" s="29" t="s">
@@ -7217,7 +7218,7 @@
         <v>266</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="29" t="s">
@@ -7242,7 +7243,7 @@
         <v>266</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D176" s="29"/>
       <c r="E176" s="29" t="s">
@@ -7267,7 +7268,7 @@
         <v>266</v>
       </c>
       <c r="C177" s="31" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D177" s="29"/>
       <c r="E177" s="29" t="s">
@@ -7292,7 +7293,7 @@
         <v>266</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D178" s="29"/>
       <c r="E178" s="29" t="s">
@@ -7317,7 +7318,7 @@
         <v>267</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D179" s="29"/>
       <c r="E179" s="29" t="s">
@@ -7342,7 +7343,7 @@
         <v>267</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D180" s="29"/>
       <c r="E180" s="29" t="s">
@@ -7367,7 +7368,7 @@
         <v>267</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D181" s="29"/>
       <c r="E181" s="29" t="s">
@@ -7392,7 +7393,7 @@
         <v>268</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D182" s="29"/>
       <c r="E182" s="29" t="s">
@@ -7417,7 +7418,7 @@
         <v>268</v>
       </c>
       <c r="C183" s="31" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D183" s="29"/>
       <c r="E183" s="29" t="s">
@@ -7442,7 +7443,7 @@
         <v>268</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="29" t="s">
@@ -7467,7 +7468,7 @@
         <v>268</v>
       </c>
       <c r="C185" s="31" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D185" s="29"/>
       <c r="E185" s="29" t="s">
@@ -7492,7 +7493,7 @@
         <v>268</v>
       </c>
       <c r="C186" s="31" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="29" t="s">
@@ -7517,7 +7518,7 @@
         <v>268</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="29" t="s">
@@ -7542,7 +7543,7 @@
         <v>268</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="29" t="s">
@@ -7567,7 +7568,7 @@
         <v>269</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D189" s="29"/>
       <c r="E189" s="29" t="s">
@@ -7592,7 +7593,7 @@
         <v>269</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D190" s="29"/>
       <c r="E190" s="29" t="s">
@@ -7617,7 +7618,7 @@
         <v>269</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D191" s="29"/>
       <c r="E191" s="29" t="s">
@@ -7642,7 +7643,7 @@
         <v>269</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D192" s="29"/>
       <c r="E192" s="29" t="s">
@@ -7667,7 +7668,7 @@
         <v>269</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D193" s="29"/>
       <c r="E193" s="29" t="s">
@@ -7692,7 +7693,7 @@
         <v>269</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D194" s="29"/>
       <c r="E194" s="29" t="s">
@@ -7717,7 +7718,7 @@
         <v>269</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D195" s="29"/>
       <c r="E195" s="29" t="s">
@@ -7742,7 +7743,7 @@
         <v>269</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -7767,7 +7768,7 @@
         <v>270</v>
       </c>
       <c r="C197" s="31" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D197" s="29"/>
       <c r="E197" s="29" t="s">
@@ -7792,7 +7793,7 @@
         <v>270</v>
       </c>
       <c r="C198" s="31" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -7817,7 +7818,7 @@
         <v>270</v>
       </c>
       <c r="C199" s="31" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D199" s="29"/>
       <c r="E199" s="29" t="s">
@@ -7842,7 +7843,7 @@
         <v>270</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D200" s="29"/>
       <c r="E200" s="29" t="s">
@@ -7867,7 +7868,7 @@
         <v>270</v>
       </c>
       <c r="C201" s="31" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -7892,7 +7893,7 @@
         <v>270</v>
       </c>
       <c r="C202" s="31" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D202" s="29"/>
       <c r="E202" s="29" t="s">
@@ -7917,7 +7918,7 @@
         <v>270</v>
       </c>
       <c r="C203" s="31" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D203" s="29"/>
       <c r="E203" s="29" t="s">
@@ -7942,7 +7943,7 @@
         <v>271</v>
       </c>
       <c r="C204" s="31" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D204" s="29"/>
       <c r="E204" s="29" t="s">
@@ -7967,7 +7968,7 @@
         <v>272</v>
       </c>
       <c r="C205" s="31" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D205" s="29"/>
       <c r="E205" s="29" t="s">
@@ -7992,7 +7993,7 @@
         <v>272</v>
       </c>
       <c r="C206" s="31" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D206" s="29"/>
       <c r="E206" s="29" t="s">
@@ -8017,7 +8018,7 @@
         <v>272</v>
       </c>
       <c r="C207" s="31" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D207" s="29"/>
       <c r="E207" s="29" t="s">
@@ -8034,15 +8035,15 @@
       </c>
       <c r="I207" s="31"/>
     </row>
-    <row r="208" spans="1:9" ht="30">
+    <row r="208" spans="1:9" ht="45">
       <c r="A208" s="29" t="s">
         <v>231</v>
       </c>
       <c r="B208" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="C208" s="31" t="s">
-        <v>461</v>
+      <c r="C208" s="20" t="s">
+        <v>505</v>
       </c>
       <c r="D208" s="29"/>
       <c r="E208" s="29" t="s">
@@ -8061,16 +8062,16 @@
     </row>
     <row r="209" spans="1:9" ht="45">
       <c r="A209" s="22" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="B209" s="30" t="s">
         <v>272</v>
       </c>
       <c r="C209" s="31" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="D209" s="29" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="E209" s="29" t="s">
         <v>22</v>
@@ -8088,16 +8089,16 @@
     </row>
     <row r="210" spans="1:9" ht="45">
       <c r="A210" s="29" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B210" s="30" t="s">
         <v>272</v>
       </c>
       <c r="C210" s="31" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="D210" s="29" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="E210" s="29" t="s">
         <v>22</v>
@@ -8112,21 +8113,21 @@
         <v>20</v>
       </c>
       <c r="I210" s="31" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="211" spans="1:9" ht="45">
       <c r="A211" s="29" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B211" s="30" t="s">
         <v>272</v>
       </c>
       <c r="C211" s="31" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="E211" s="29" t="s">
         <v>22</v>
@@ -8141,21 +8142,21 @@
         <v>20</v>
       </c>
       <c r="I211" s="31" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="212" spans="1:9" ht="60">
       <c r="A212" s="29" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="B212" s="30" t="s">
         <v>272</v>
       </c>
       <c r="C212" s="31" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="E212" s="29" t="s">
         <v>22</v>
@@ -8170,7 +8171,7 @@
         <v>20</v>
       </c>
       <c r="I212" s="31" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="213" spans="1:9" ht="105">
@@ -8180,7 +8181,7 @@
       <c r="B213" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="C213" s="31" t="s">
+      <c r="C213" s="20" t="s">
         <v>506</v>
       </c>
       <c r="D213" s="29"/>
@@ -8206,7 +8207,7 @@
         <v>272</v>
       </c>
       <c r="C214" s="31" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="D214" s="29"/>
       <c r="E214" s="29" t="s">
@@ -8231,7 +8232,7 @@
         <v>272</v>
       </c>
       <c r="C215" s="31" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D215" s="29"/>
       <c r="E215" s="29" t="s">
@@ -8247,7 +8248,7 @@
         <v>21</v>
       </c>
       <c r="I215" s="31" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -8258,7 +8259,7 @@
         <v>273</v>
       </c>
       <c r="C216" s="31" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D216" s="29"/>
       <c r="E216" s="29" t="s">
@@ -8283,7 +8284,7 @@
         <v>273</v>
       </c>
       <c r="C217" s="31" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D217" s="29"/>
       <c r="E217" s="29" t="s">
@@ -8308,7 +8309,7 @@
         <v>274</v>
       </c>
       <c r="C218" s="31" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D218" s="29"/>
       <c r="E218" s="29" t="s">
@@ -8333,7 +8334,7 @@
         <v>274</v>
       </c>
       <c r="C219" s="31" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D219" s="29"/>
       <c r="E219" s="29" t="s">
@@ -8358,7 +8359,7 @@
         <v>275</v>
       </c>
       <c r="C220" s="31" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D220" s="29"/>
       <c r="E220" s="29" t="s">
@@ -8383,7 +8384,7 @@
         <v>275</v>
       </c>
       <c r="C221" s="31" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D221" s="29"/>
       <c r="E221" s="29" t="s">
@@ -8408,7 +8409,7 @@
         <v>276</v>
       </c>
       <c r="C222" s="31" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D222" s="29"/>
       <c r="E222" s="29" t="s">
@@ -8433,7 +8434,7 @@
         <v>276</v>
       </c>
       <c r="C223" s="31" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D223" s="29"/>
       <c r="E223" s="29" t="s">
@@ -8458,7 +8459,7 @@
         <v>277</v>
       </c>
       <c r="C224" s="31" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D224" s="29"/>
       <c r="E224" s="29" t="s">
@@ -8483,7 +8484,7 @@
         <v>278</v>
       </c>
       <c r="C225" s="31" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D225" s="29"/>
       <c r="E225" s="29" t="s">
@@ -8508,7 +8509,7 @@
         <v>278</v>
       </c>
       <c r="C226" s="31" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D226" s="29"/>
       <c r="E226" s="29" t="s">
@@ -8533,7 +8534,7 @@
         <v>279</v>
       </c>
       <c r="C227" s="31" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D227" s="29"/>
       <c r="E227" s="29" t="s">
@@ -8558,7 +8559,7 @@
         <v>279</v>
       </c>
       <c r="C228" s="31" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D228" s="29"/>
       <c r="E228" s="29" t="s">
@@ -8583,7 +8584,7 @@
         <v>279</v>
       </c>
       <c r="C229" s="31" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D229" s="29"/>
       <c r="E229" s="29" t="s">
@@ -8608,7 +8609,7 @@
         <v>280</v>
       </c>
       <c r="C230" s="31" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D230" s="29"/>
       <c r="E230" s="29" t="s">
@@ -8633,7 +8634,7 @@
         <v>280</v>
       </c>
       <c r="C231" s="31" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D231" s="29"/>
       <c r="E231" s="29" t="s">
@@ -8660,6 +8661,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -8667,11 +8673,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H231 A34:I231">
@@ -8727,20 +8728,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F231">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F231" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E231">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E231" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G231">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G231" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H231">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H231" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8750,7 +8751,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B212:B233 B19:B211 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B212:B233 B19:B211" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -8760,6 +8761,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -8808,12 +8815,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8824,6 +8825,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8838,20 +8853,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Update MS-OXCPERM RS Description
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCPERM/MS-OXCPERM_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCPERM/MS-OXCPERM_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE79AFE9-3AE9-4F6A-AE90-77B4442EA707}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A270249-7EF6-450A-9FD5-DE1713BC785E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -939,12 +939,6 @@
     <t>MS-OXCPERM_R1179</t>
   </si>
   <si>
-    <t>MS-OXCPERM_R1180</t>
-  </si>
-  <si>
-    <t>MS-OXCPERM_R1182</t>
-  </si>
-  <si>
     <t>MS-OXCPERM_R1183</t>
   </si>
   <si>
@@ -1764,13 +1758,23 @@
     <t>[In PidTagMemberRights Property] The PidTagMemberRights property ([MS-OXPROPS] section 2.778) specifies the folder permissions that are granted to the specified user.</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] &lt;2&gt; Section 2.2.3: Outlook 2010, Outlook 2013, Outlook 2016, Outlook 2019 Preview  do not use the PidTagAccessControlListData property (section 2.2.3).</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] &lt;5&gt; Section 2.2.7: Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview include the FreeBusySimple flag by default on the Calendar folder for any entry in the permissions list except the anonymous user and add the FreeBusyDetailed flag to any entries that have the ReadAny flag set. Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 Preview use these defaults until the client modifies the permissions list with the IncludeFreeBusy flag set in the RopModifyPermissions ROP request to override the default value.</t>
-  </si>
-  <si>
     <t>12.0</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] &lt;2&gt; Section 2.2.3: Outlook 2010, Outlook 2013, Outlook 2016, Outlook 2019  do not use the PidTagAccessControlListData property (section 2.2.3).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXCPERM_R1180</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] &lt;5&gt; Section 2.2.7: Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 include the FreeBusySimple flag by default on the Calendar folder for any entry in the permissions list except the anonymous user and add the FreeBusyDetailed flag to any entries that have the ReadAny flag set. Exchange 2007, Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 use these defaults until the client modifies the permissions list with the IncludeFreeBusy flag set in the RopModifyPermissions ROP request to override the default value.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXCPERM_R1182</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1778,14 +1782,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1825,6 +1829,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1981,13 +1986,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2020,7 +2025,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2083,7 +2088,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="33">
     <dxf>
@@ -2627,31 +2632,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I231" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Normal" dataCellStyle="Normal" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I231" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I231" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16" dataCellStyle="Normal">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15" dataCellStyle="Normal">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14" dataCellStyle="Normal">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13" dataCellStyle="Normal">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12" dataCellStyle="Normal">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11" dataCellStyle="Normal">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10" dataCellStyle="Normal">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9" dataCellStyle="Normal">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
@@ -2675,7 +2680,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3000,23 +3005,23 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="25.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="100.125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -3024,9 +3029,9 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3035,12 +3040,12 @@
       <c r="F2" s="25"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -3050,7 +3055,7 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="21">
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -3062,7 +3067,7 @@
       <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
@@ -3078,7 +3083,7 @@
       <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
@@ -3094,7 +3099,7 @@
       <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -3110,7 +3115,7 @@
       <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
@@ -3126,7 +3131,7 @@
       <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="78.75" customHeight="1">
+    <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
@@ -3142,7 +3147,7 @@
       <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="33.75" customHeight="1">
+    <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
@@ -3158,7 +3163,7 @@
       <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
@@ -3174,7 +3179,7 @@
       <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
@@ -3192,7 +3197,7 @@
       <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
@@ -3210,7 +3215,7 @@
       <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>7</v>
       </c>
@@ -3228,7 +3233,7 @@
       <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>3</v>
       </c>
@@ -3246,7 +3251,7 @@
       <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1">
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
@@ -3262,7 +3267,7 @@
       <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="64.5" customHeight="1">
+    <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
@@ -3278,7 +3283,7 @@
       <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -3295,7 +3300,7 @@
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30">
+    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -3325,15 +3330,15 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="20" spans="1:12" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22" t="s">
@@ -3350,15 +3355,15 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1">
+    <row r="21" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="s">
@@ -3375,15 +3380,15 @@
       </c>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A22" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="s">
@@ -3400,15 +3405,15 @@
       </c>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="23" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A23" s="22" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22" t="s">
@@ -3425,15 +3430,15 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A24" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22" t="s">
@@ -3450,15 +3455,15 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="25" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A25" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
@@ -3475,15 +3480,15 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="26" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
@@ -3500,15 +3505,15 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="27" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A27" s="22" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22" t="s">
@@ -3525,15 +3530,15 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22" t="s">
@@ -3550,15 +3555,15 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A29" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22" t="s">
@@ -3574,18 +3579,18 @@
         <v>17</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" s="23" customFormat="1" ht="30">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A30" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -3602,15 +3607,15 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="31" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A31" s="22" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22" t="s">
@@ -3627,15 +3632,15 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1">
+    <row r="32" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A32" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
@@ -3652,15 +3657,15 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" ht="45">
+    <row r="33" spans="1:9" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A33" s="22" t="s">
         <v>56</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22" t="s">
@@ -3677,15 +3682,15 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" ht="45">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="29" t="s">
@@ -3702,15 +3707,15 @@
       </c>
       <c r="I34" s="31"/>
     </row>
-    <row r="35" spans="1:9" ht="45">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29" t="s">
@@ -3727,15 +3732,15 @@
       </c>
       <c r="I35" s="31"/>
     </row>
-    <row r="36" spans="1:9" ht="30">
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29" t="s">
@@ -3752,15 +3757,15 @@
       </c>
       <c r="I36" s="31"/>
     </row>
-    <row r="37" spans="1:9" ht="30">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
         <v>60</v>
       </c>
       <c r="B37" s="30" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29" t="s">
@@ -3777,15 +3782,15 @@
       </c>
       <c r="I37" s="31"/>
     </row>
-    <row r="38" spans="1:9" ht="45">
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
         <v>61</v>
       </c>
       <c r="B38" s="30" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29" t="s">
@@ -3802,15 +3807,15 @@
       </c>
       <c r="I38" s="31"/>
     </row>
-    <row r="39" spans="1:9" ht="30">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
         <v>62</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29" t="s">
@@ -3827,15 +3832,15 @@
       </c>
       <c r="I39" s="31"/>
     </row>
-    <row r="40" spans="1:9" ht="30">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
         <v>63</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="29" t="s">
@@ -3852,15 +3857,15 @@
       </c>
       <c r="I40" s="31"/>
     </row>
-    <row r="41" spans="1:9" ht="30">
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
         <v>64</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="29" t="s">
@@ -3877,15 +3882,15 @@
       </c>
       <c r="I41" s="31"/>
     </row>
-    <row r="42" spans="1:9" ht="75">
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
         <v>65</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="29" t="s">
@@ -3901,18 +3906,18 @@
         <v>17</v>
       </c>
       <c r="I42" s="31" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="30">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29" t="s">
@@ -3929,15 +3934,15 @@
       </c>
       <c r="I43" s="31"/>
     </row>
-    <row r="44" spans="1:9" ht="30">
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
         <v>67</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29" t="s">
@@ -3954,15 +3959,15 @@
       </c>
       <c r="I44" s="31"/>
     </row>
-    <row r="45" spans="1:9" ht="30">
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
         <v>68</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29" t="s">
@@ -3979,15 +3984,15 @@
       </c>
       <c r="I45" s="31"/>
     </row>
-    <row r="46" spans="1:9" ht="150">
+    <row r="46" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
         <v>69</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29" t="s">
@@ -4003,18 +4008,18 @@
         <v>17</v>
       </c>
       <c r="I46" s="31" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="30">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
         <v>70</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29" t="s">
@@ -4031,15 +4036,15 @@
       </c>
       <c r="I47" s="31"/>
     </row>
-    <row r="48" spans="1:9" ht="30">
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
         <v>71</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="29" t="s">
@@ -4056,15 +4061,15 @@
       </c>
       <c r="I48" s="31"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
         <v>72</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="29" t="s">
@@ -4081,15 +4086,15 @@
       </c>
       <c r="I49" s="31"/>
     </row>
-    <row r="50" spans="1:9" ht="45">
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
         <v>73</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="29" t="s">
@@ -4106,15 +4111,15 @@
       </c>
       <c r="I50" s="31"/>
     </row>
-    <row r="51" spans="1:9" ht="30">
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
         <v>74</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D51" s="29"/>
       <c r="E51" s="29" t="s">
@@ -4131,15 +4136,15 @@
       </c>
       <c r="I51" s="31"/>
     </row>
-    <row r="52" spans="1:9" ht="60">
+    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="29" t="s">
         <v>75</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D52" s="29"/>
       <c r="E52" s="29" t="s">
@@ -4156,15 +4161,15 @@
       </c>
       <c r="I52" s="31"/>
     </row>
-    <row r="53" spans="1:9" ht="60">
+    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="29" t="s">
         <v>76</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="29" t="s">
@@ -4181,15 +4186,15 @@
       </c>
       <c r="I53" s="31"/>
     </row>
-    <row r="54" spans="1:9" ht="60">
+    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
         <v>77</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D54" s="29"/>
       <c r="E54" s="29" t="s">
@@ -4206,15 +4211,15 @@
       </c>
       <c r="I54" s="31"/>
     </row>
-    <row r="55" spans="1:9" ht="45">
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
         <v>78</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29" t="s">
@@ -4231,15 +4236,15 @@
       </c>
       <c r="I55" s="31"/>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
         <v>79</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D56" s="29"/>
       <c r="E56" s="29" t="s">
@@ -4256,15 +4261,15 @@
       </c>
       <c r="I56" s="31"/>
     </row>
-    <row r="57" spans="1:9" ht="45">
+    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="29" t="s">
         <v>80</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D57" s="29"/>
       <c r="E57" s="29" t="s">
@@ -4281,15 +4286,15 @@
       </c>
       <c r="I57" s="31"/>
     </row>
-    <row r="58" spans="1:9" ht="30">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="29" t="s">
         <v>81</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D58" s="29"/>
       <c r="E58" s="29" t="s">
@@ -4306,15 +4311,15 @@
       </c>
       <c r="I58" s="31"/>
     </row>
-    <row r="59" spans="1:9" ht="30">
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="29" t="s">
         <v>82</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29" t="s">
@@ -4331,15 +4336,15 @@
       </c>
       <c r="I59" s="31"/>
     </row>
-    <row r="60" spans="1:9" ht="30">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="29" t="s">
         <v>83</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="29" t="s">
@@ -4356,15 +4361,15 @@
       </c>
       <c r="I60" s="31"/>
     </row>
-    <row r="61" spans="1:9" ht="30">
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="29" t="s">
         <v>84</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D61" s="29"/>
       <c r="E61" s="29" t="s">
@@ -4381,15 +4386,15 @@
       </c>
       <c r="I61" s="31"/>
     </row>
-    <row r="62" spans="1:9" ht="30">
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
         <v>85</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="29" t="s">
@@ -4406,15 +4411,15 @@
       </c>
       <c r="I62" s="31"/>
     </row>
-    <row r="63" spans="1:9" ht="30">
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="29" t="s">
         <v>86</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29" t="s">
@@ -4431,15 +4436,15 @@
       </c>
       <c r="I63" s="31"/>
     </row>
-    <row r="64" spans="1:9" ht="45">
+    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="29" t="s">
         <v>87</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29" t="s">
@@ -4456,15 +4461,15 @@
       </c>
       <c r="I64" s="31"/>
     </row>
-    <row r="65" spans="1:9" ht="30">
+    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="29" t="s">
         <v>88</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29" t="s">
@@ -4481,15 +4486,15 @@
       </c>
       <c r="I65" s="31"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="29" t="s">
         <v>89</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="29" t="s">
@@ -4506,15 +4511,15 @@
       </c>
       <c r="I66" s="31"/>
     </row>
-    <row r="67" spans="1:9" ht="45">
+    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="s">
         <v>90</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29" t="s">
@@ -4531,15 +4536,15 @@
       </c>
       <c r="I67" s="31"/>
     </row>
-    <row r="68" spans="1:9" ht="45">
+    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
         <v>91</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -4556,15 +4561,15 @@
       </c>
       <c r="I68" s="31"/>
     </row>
-    <row r="69" spans="1:9" ht="30">
+    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
         <v>92</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -4581,15 +4586,15 @@
       </c>
       <c r="I69" s="31"/>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
         <v>93</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="29" t="s">
@@ -4606,15 +4611,15 @@
       </c>
       <c r="I70" s="31"/>
     </row>
-    <row r="71" spans="1:9" ht="30">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
         <v>94</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D71" s="29"/>
       <c r="E71" s="29" t="s">
@@ -4631,15 +4636,15 @@
       </c>
       <c r="I71" s="31"/>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
         <v>95</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D72" s="29"/>
       <c r="E72" s="29" t="s">
@@ -4656,15 +4661,15 @@
       </c>
       <c r="I72" s="31"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
         <v>96</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C73" s="31" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29" t="s">
@@ -4681,15 +4686,15 @@
       </c>
       <c r="I73" s="31"/>
     </row>
-    <row r="74" spans="1:9" ht="30">
+    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
         <v>97</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="29" t="s">
@@ -4706,15 +4711,15 @@
       </c>
       <c r="I74" s="31"/>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="29" t="s">
         <v>98</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D75" s="29"/>
       <c r="E75" s="29" t="s">
@@ -4731,15 +4736,15 @@
       </c>
       <c r="I75" s="31"/>
     </row>
-    <row r="76" spans="1:9" ht="30">
+    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="29" t="s">
         <v>99</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D76" s="29"/>
       <c r="E76" s="29" t="s">
@@ -4756,15 +4761,15 @@
       </c>
       <c r="I76" s="31"/>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="29" t="s">
         <v>100</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D77" s="29"/>
       <c r="E77" s="29" t="s">
@@ -4781,15 +4786,15 @@
       </c>
       <c r="I77" s="31"/>
     </row>
-    <row r="78" spans="1:9" ht="30">
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="29" t="s">
         <v>101</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D78" s="29"/>
       <c r="E78" s="29" t="s">
@@ -4806,15 +4811,15 @@
       </c>
       <c r="I78" s="31"/>
     </row>
-    <row r="79" spans="1:9" ht="30">
+    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="29" t="s">
         <v>102</v>
       </c>
       <c r="B79" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D79" s="29"/>
       <c r="E79" s="29" t="s">
@@ -4831,15 +4836,15 @@
       </c>
       <c r="I79" s="31"/>
     </row>
-    <row r="80" spans="1:9" ht="30">
+    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="29" t="s">
         <v>103</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D80" s="29"/>
       <c r="E80" s="29" t="s">
@@ -4856,15 +4861,15 @@
       </c>
       <c r="I80" s="31"/>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="29" t="s">
         <v>104</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D81" s="29"/>
       <c r="E81" s="29" t="s">
@@ -4881,15 +4886,15 @@
       </c>
       <c r="I81" s="31"/>
     </row>
-    <row r="82" spans="1:9" ht="30">
+    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="29" t="s">
         <v>105</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C82" s="31" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D82" s="29"/>
       <c r="E82" s="29" t="s">
@@ -4906,15 +4911,15 @@
       </c>
       <c r="I82" s="31"/>
     </row>
-    <row r="83" spans="1:9" ht="45">
+    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="29" t="s">
         <v>106</v>
       </c>
       <c r="B83" s="30" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D83" s="29"/>
       <c r="E83" s="29" t="s">
@@ -4931,15 +4936,15 @@
       </c>
       <c r="I83" s="31"/>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="29" t="s">
         <v>107</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D84" s="29"/>
       <c r="E84" s="29" t="s">
@@ -4956,15 +4961,15 @@
       </c>
       <c r="I84" s="31"/>
     </row>
-    <row r="85" spans="1:9" ht="30">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="29" t="s">
         <v>108</v>
       </c>
       <c r="B85" s="30" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D85" s="29"/>
       <c r="E85" s="29" t="s">
@@ -4981,15 +4986,15 @@
       </c>
       <c r="I85" s="31"/>
     </row>
-    <row r="86" spans="1:9" ht="30">
+    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="29" t="s">
         <v>109</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C86" s="31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D86" s="29"/>
       <c r="E86" s="29" t="s">
@@ -5006,15 +5011,15 @@
       </c>
       <c r="I86" s="31"/>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="29" t="s">
         <v>110</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D87" s="29"/>
       <c r="E87" s="29" t="s">
@@ -5031,15 +5036,15 @@
       </c>
       <c r="I87" s="31"/>
     </row>
-    <row r="88" spans="1:9" ht="45">
+    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="29" t="s">
         <v>111</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="29" t="s">
@@ -5056,15 +5061,15 @@
       </c>
       <c r="I88" s="31"/>
     </row>
-    <row r="89" spans="1:9" ht="30">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="29" t="s">
         <v>112</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C89" s="31" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="29" t="s">
@@ -5081,15 +5086,15 @@
       </c>
       <c r="I89" s="31"/>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="29" t="s">
         <v>113</v>
       </c>
       <c r="B90" s="30" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C90" s="31" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="29" t="s">
@@ -5106,15 +5111,15 @@
       </c>
       <c r="I90" s="31"/>
     </row>
-    <row r="91" spans="1:9" ht="30">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="29" t="s">
         <v>114</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="29" t="s">
@@ -5131,15 +5136,15 @@
       </c>
       <c r="I91" s="31"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="29" t="s">
         <v>115</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D92" s="29"/>
       <c r="E92" s="29" t="s">
@@ -5156,15 +5161,15 @@
       </c>
       <c r="I92" s="31"/>
     </row>
-    <row r="93" spans="1:9" ht="30">
+    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="29" t="s">
         <v>116</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D93" s="29"/>
       <c r="E93" s="29" t="s">
@@ -5181,15 +5186,15 @@
       </c>
       <c r="I93" s="31"/>
     </row>
-    <row r="94" spans="1:9" ht="30">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="29" t="s">
         <v>117</v>
       </c>
       <c r="B94" s="30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C94" s="31" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D94" s="29"/>
       <c r="E94" s="29" t="s">
@@ -5206,15 +5211,15 @@
       </c>
       <c r="I94" s="31"/>
     </row>
-    <row r="95" spans="1:9" ht="45">
+    <row r="95" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="29" t="s">
         <v>118</v>
       </c>
       <c r="B95" s="30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D95" s="29"/>
       <c r="E95" s="29" t="s">
@@ -5231,15 +5236,15 @@
       </c>
       <c r="I95" s="31"/>
     </row>
-    <row r="96" spans="1:9" ht="45">
+    <row r="96" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
         <v>119</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C96" s="31" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D96" s="29"/>
       <c r="E96" s="29" t="s">
@@ -5256,15 +5261,15 @@
       </c>
       <c r="I96" s="31"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="29" t="s">
         <v>120</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D97" s="29"/>
       <c r="E97" s="29" t="s">
@@ -5281,15 +5286,15 @@
       </c>
       <c r="I97" s="31"/>
     </row>
-    <row r="98" spans="1:9" ht="30">
+    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="29" t="s">
         <v>121</v>
       </c>
       <c r="B98" s="30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C98" s="20" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D98" s="29"/>
       <c r="E98" s="29" t="s">
@@ -5306,15 +5311,15 @@
       </c>
       <c r="I98" s="31"/>
     </row>
-    <row r="99" spans="1:9" ht="30">
+    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" s="29" t="s">
         <v>122</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C99" s="31" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D99" s="29"/>
       <c r="E99" s="29" t="s">
@@ -5331,15 +5336,15 @@
       </c>
       <c r="I99" s="31"/>
     </row>
-    <row r="100" spans="1:9" ht="30">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="29" t="s">
         <v>123</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C100" s="31" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D100" s="29"/>
       <c r="E100" s="29" t="s">
@@ -5356,15 +5361,15 @@
       </c>
       <c r="I100" s="31"/>
     </row>
-    <row r="101" spans="1:9" ht="30">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="29" t="s">
         <v>124</v>
       </c>
       <c r="B101" s="30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C101" s="31" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D101" s="29"/>
       <c r="E101" s="29" t="s">
@@ -5381,15 +5386,15 @@
       </c>
       <c r="I101" s="31"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
         <v>125</v>
       </c>
       <c r="B102" s="30" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C102" s="31" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D102" s="29"/>
       <c r="E102" s="29" t="s">
@@ -5406,15 +5411,15 @@
       </c>
       <c r="I102" s="31"/>
     </row>
-    <row r="103" spans="1:9" ht="30">
+    <row r="103" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="29" t="s">
         <v>126</v>
       </c>
       <c r="B103" s="30" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C103" s="20" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D103" s="29"/>
       <c r="E103" s="29" t="s">
@@ -5431,15 +5436,15 @@
       </c>
       <c r="I103" s="31"/>
     </row>
-    <row r="104" spans="1:9" ht="30">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="29" t="s">
         <v>127</v>
       </c>
       <c r="B104" s="30" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C104" s="31" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D104" s="29"/>
       <c r="E104" s="29" t="s">
@@ -5456,15 +5461,15 @@
       </c>
       <c r="I104" s="31"/>
     </row>
-    <row r="105" spans="1:9" ht="45">
+    <row r="105" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="29" t="s">
         <v>128</v>
       </c>
       <c r="B105" s="30" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C105" s="31" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D105" s="29"/>
       <c r="E105" s="29" t="s">
@@ -5481,15 +5486,15 @@
       </c>
       <c r="I105" s="31"/>
     </row>
-    <row r="106" spans="1:9" ht="30">
+    <row r="106" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="29" t="s">
         <v>129</v>
       </c>
       <c r="B106" s="30" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C106" s="31" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D106" s="29"/>
       <c r="E106" s="29" t="s">
@@ -5506,15 +5511,15 @@
       </c>
       <c r="I106" s="31"/>
     </row>
-    <row r="107" spans="1:9" ht="30">
+    <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="29" t="s">
         <v>130</v>
       </c>
       <c r="B107" s="30" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="29" t="s">
@@ -5531,15 +5536,15 @@
       </c>
       <c r="I107" s="31"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="29" t="s">
         <v>131</v>
       </c>
       <c r="B108" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D108" s="29"/>
       <c r="E108" s="29" t="s">
@@ -5556,15 +5561,15 @@
       </c>
       <c r="I108" s="31"/>
     </row>
-    <row r="109" spans="1:9" ht="30">
+    <row r="109" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="29" t="s">
         <v>132</v>
       </c>
       <c r="B109" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D109" s="29"/>
       <c r="E109" s="29" t="s">
@@ -5581,15 +5586,15 @@
       </c>
       <c r="I109" s="31"/>
     </row>
-    <row r="110" spans="1:9" ht="30">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="29" t="s">
         <v>133</v>
       </c>
       <c r="B110" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D110" s="29"/>
       <c r="E110" s="29" t="s">
@@ -5606,15 +5611,15 @@
       </c>
       <c r="I110" s="31"/>
     </row>
-    <row r="111" spans="1:9" ht="45">
+    <row r="111" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="29" t="s">
         <v>134</v>
       </c>
       <c r="B111" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D111" s="29"/>
       <c r="E111" s="29" t="s">
@@ -5631,15 +5636,15 @@
       </c>
       <c r="I111" s="31"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="29" t="s">
         <v>135</v>
       </c>
       <c r="B112" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="29" t="s">
@@ -5656,15 +5661,15 @@
       </c>
       <c r="I112" s="31"/>
     </row>
-    <row r="113" spans="1:9" ht="30">
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="29" t="s">
         <v>136</v>
       </c>
       <c r="B113" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D113" s="29"/>
       <c r="E113" s="29" t="s">
@@ -5681,15 +5686,15 @@
       </c>
       <c r="I113" s="31"/>
     </row>
-    <row r="114" spans="1:9" ht="30">
+    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="29" t="s">
         <v>137</v>
       </c>
       <c r="B114" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C114" s="31" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="29" t="s">
@@ -5706,15 +5711,15 @@
       </c>
       <c r="I114" s="31"/>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="29" t="s">
         <v>138</v>
       </c>
       <c r="B115" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C115" s="31" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -5731,15 +5736,15 @@
       </c>
       <c r="I115" s="31"/>
     </row>
-    <row r="116" spans="1:9" ht="30">
+    <row r="116" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="29" t="s">
         <v>139</v>
       </c>
       <c r="B116" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C116" s="31" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="29" t="s">
@@ -5756,15 +5761,15 @@
       </c>
       <c r="I116" s="31"/>
     </row>
-    <row r="117" spans="1:9" ht="30">
+    <row r="117" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="29" t="s">
         <v>140</v>
       </c>
       <c r="B117" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C117" s="31" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="29" t="s">
@@ -5781,15 +5786,15 @@
       </c>
       <c r="I117" s="31"/>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="29" t="s">
         <v>141</v>
       </c>
       <c r="B118" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="29" t="s">
@@ -5806,15 +5811,15 @@
       </c>
       <c r="I118" s="31"/>
     </row>
-    <row r="119" spans="1:9" ht="45">
+    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="29" t="s">
         <v>142</v>
       </c>
       <c r="B119" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C119" s="31" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="29" t="s">
@@ -5831,15 +5836,15 @@
       </c>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="1:9" ht="30">
+    <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="29" t="s">
         <v>143</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C120" s="31" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D120" s="29"/>
       <c r="E120" s="29" t="s">
@@ -5856,15 +5861,15 @@
       </c>
       <c r="I120" s="31"/>
     </row>
-    <row r="121" spans="1:9" ht="30">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="29" t="s">
         <v>144</v>
       </c>
       <c r="B121" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C121" s="31" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="29" t="s">
@@ -5881,15 +5886,15 @@
       </c>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="29" t="s">
         <v>145</v>
       </c>
       <c r="B122" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C122" s="31" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="29" t="s">
@@ -5906,15 +5911,15 @@
       </c>
       <c r="I122" s="31"/>
     </row>
-    <row r="123" spans="1:9" ht="45">
+    <row r="123" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="29" t="s">
         <v>146</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C123" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29" t="s">
@@ -5931,15 +5936,15 @@
       </c>
       <c r="I123" s="31"/>
     </row>
-    <row r="124" spans="1:9" ht="30">
+    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="29" t="s">
         <v>147</v>
       </c>
       <c r="B124" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C124" s="31" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D124" s="29"/>
       <c r="E124" s="29" t="s">
@@ -5956,15 +5961,15 @@
       </c>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="1:9" ht="30">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="29" t="s">
         <v>148</v>
       </c>
       <c r="B125" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C125" s="31" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="29" t="s">
@@ -5981,15 +5986,15 @@
       </c>
       <c r="I125" s="31"/>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="29" t="s">
         <v>149</v>
       </c>
       <c r="B126" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C126" s="31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="29" t="s">
@@ -6006,15 +6011,15 @@
       </c>
       <c r="I126" s="31"/>
     </row>
-    <row r="127" spans="1:9" ht="30">
+    <row r="127" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="29" t="s">
         <v>150</v>
       </c>
       <c r="B127" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C127" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="29" t="s">
@@ -6031,15 +6036,15 @@
       </c>
       <c r="I127" s="31"/>
     </row>
-    <row r="128" spans="1:9" ht="30">
+    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="29" t="s">
         <v>151</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C128" s="31" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="29" t="s">
@@ -6056,15 +6061,15 @@
       </c>
       <c r="I128" s="31"/>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="29" t="s">
         <v>152</v>
       </c>
       <c r="B129" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C129" s="31" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="29" t="s">
@@ -6081,15 +6086,15 @@
       </c>
       <c r="I129" s="31"/>
     </row>
-    <row r="130" spans="1:9" ht="30">
+    <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="29" t="s">
         <v>153</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C130" s="31" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="29" t="s">
@@ -6106,15 +6111,15 @@
       </c>
       <c r="I130" s="31"/>
     </row>
-    <row r="131" spans="1:9" ht="30">
+    <row r="131" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="29" t="s">
         <v>154</v>
       </c>
       <c r="B131" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C131" s="31" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -6131,15 +6136,15 @@
       </c>
       <c r="I131" s="31"/>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="29" t="s">
         <v>155</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C132" s="31" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="29" t="s">
@@ -6156,15 +6161,15 @@
       </c>
       <c r="I132" s="31"/>
     </row>
-    <row r="133" spans="1:9" ht="30">
+    <row r="133" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="29" t="s">
         <v>156</v>
       </c>
       <c r="B133" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D133" s="29"/>
       <c r="E133" s="29" t="s">
@@ -6181,15 +6186,15 @@
       </c>
       <c r="I133" s="31"/>
     </row>
-    <row r="134" spans="1:9" ht="30">
+    <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="29" t="s">
         <v>157</v>
       </c>
       <c r="B134" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C134" s="31" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="29" t="s">
@@ -6206,15 +6211,15 @@
       </c>
       <c r="I134" s="31"/>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="29" t="s">
         <v>158</v>
       </c>
       <c r="B135" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C135" s="31" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="29" t="s">
@@ -6231,15 +6236,15 @@
       </c>
       <c r="I135" s="31"/>
     </row>
-    <row r="136" spans="1:9" ht="45">
+    <row r="136" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="29" t="s">
         <v>159</v>
       </c>
       <c r="B136" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C136" s="31" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="29" t="s">
@@ -6255,18 +6260,18 @@
         <v>17</v>
       </c>
       <c r="I136" s="20" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" ht="60">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="29" t="s">
         <v>160</v>
       </c>
       <c r="B137" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C137" s="31" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="29" t="s">
@@ -6282,18 +6287,18 @@
         <v>17</v>
       </c>
       <c r="I137" s="31" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="29" t="s">
         <v>161</v>
       </c>
       <c r="B138" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C138" s="31" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="29" t="s">
@@ -6310,15 +6315,15 @@
       </c>
       <c r="I138" s="31"/>
     </row>
-    <row r="139" spans="1:9" ht="30">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="29" t="s">
         <v>162</v>
       </c>
       <c r="B139" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C139" s="31" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="29" t="s">
@@ -6335,15 +6340,15 @@
       </c>
       <c r="I139" s="31"/>
     </row>
-    <row r="140" spans="1:9" ht="30">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="29" t="s">
         <v>163</v>
       </c>
       <c r="B140" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C140" s="31" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="29" t="s">
@@ -6360,15 +6365,15 @@
       </c>
       <c r="I140" s="31"/>
     </row>
-    <row r="141" spans="1:9" ht="30">
+    <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="29" t="s">
         <v>164</v>
       </c>
       <c r="B141" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C141" s="31" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="29" t="s">
@@ -6385,15 +6390,15 @@
       </c>
       <c r="I141" s="31"/>
     </row>
-    <row r="142" spans="1:9" ht="45">
+    <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" s="29" t="s">
         <v>165</v>
       </c>
       <c r="B142" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C142" s="31" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D142" s="29"/>
       <c r="E142" s="29" t="s">
@@ -6410,15 +6415,15 @@
       </c>
       <c r="I142" s="31"/>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="29" t="s">
         <v>166</v>
       </c>
       <c r="B143" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C143" s="31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -6435,15 +6440,15 @@
       </c>
       <c r="I143" s="31"/>
     </row>
-    <row r="144" spans="1:9" ht="45">
+    <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A144" s="29" t="s">
         <v>167</v>
       </c>
       <c r="B144" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C144" s="31" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="29" t="s">
@@ -6460,15 +6465,15 @@
       </c>
       <c r="I144" s="31"/>
     </row>
-    <row r="145" spans="1:9" ht="45">
+    <row r="145" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="29" t="s">
         <v>168</v>
       </c>
       <c r="B145" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C145" s="31" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D145" s="29"/>
       <c r="E145" s="29" t="s">
@@ -6485,15 +6490,15 @@
       </c>
       <c r="I145" s="31"/>
     </row>
-    <row r="146" spans="1:9" ht="30">
+    <row r="146" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="29" t="s">
         <v>169</v>
       </c>
       <c r="B146" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C146" s="31" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D146" s="29"/>
       <c r="E146" s="29" t="s">
@@ -6510,15 +6515,15 @@
       </c>
       <c r="I146" s="31"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="29" t="s">
         <v>170</v>
       </c>
       <c r="B147" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C147" s="31" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D147" s="29"/>
       <c r="E147" s="29" t="s">
@@ -6535,15 +6540,15 @@
       </c>
       <c r="I147" s="31"/>
     </row>
-    <row r="148" spans="1:9" ht="45">
+    <row r="148" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A148" s="29" t="s">
         <v>171</v>
       </c>
       <c r="B148" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C148" s="31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D148" s="29"/>
       <c r="E148" s="29" t="s">
@@ -6560,15 +6565,15 @@
       </c>
       <c r="I148" s="31"/>
     </row>
-    <row r="149" spans="1:9" ht="45">
+    <row r="149" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="29" t="s">
         <v>172</v>
       </c>
       <c r="B149" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C149" s="20" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D149" s="29"/>
       <c r="E149" s="29" t="s">
@@ -6585,15 +6590,15 @@
       </c>
       <c r="I149" s="31"/>
     </row>
-    <row r="150" spans="1:9" ht="30">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="29" t="s">
         <v>173</v>
       </c>
       <c r="B150" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C150" s="31" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="29" t="s">
@@ -6610,15 +6615,15 @@
       </c>
       <c r="I150" s="31"/>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="29" t="s">
         <v>174</v>
       </c>
       <c r="B151" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C151" s="31" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D151" s="29"/>
       <c r="E151" s="29" t="s">
@@ -6635,15 +6640,15 @@
       </c>
       <c r="I151" s="31"/>
     </row>
-    <row r="152" spans="1:9" ht="45">
+    <row r="152" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="29" t="s">
         <v>175</v>
       </c>
       <c r="B152" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C152" s="31" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="29" t="s">
@@ -6660,15 +6665,15 @@
       </c>
       <c r="I152" s="31"/>
     </row>
-    <row r="153" spans="1:9" ht="30">
+    <row r="153" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="29" t="s">
         <v>176</v>
       </c>
       <c r="B153" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C153" s="31" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="29" t="s">
@@ -6685,15 +6690,15 @@
       </c>
       <c r="I153" s="31"/>
     </row>
-    <row r="154" spans="1:9" ht="30">
+    <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="29" t="s">
         <v>177</v>
       </c>
       <c r="B154" s="30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C154" s="31" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="29" t="s">
@@ -6710,15 +6715,15 @@
       </c>
       <c r="I154" s="31"/>
     </row>
-    <row r="155" spans="1:9" ht="30">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="29" t="s">
         <v>178</v>
       </c>
       <c r="B155" s="30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C155" s="31" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="29" t="s">
@@ -6735,15 +6740,15 @@
       </c>
       <c r="I155" s="31"/>
     </row>
-    <row r="156" spans="1:9" ht="45">
+    <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="29" t="s">
         <v>179</v>
       </c>
       <c r="B156" s="30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C156" s="31" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="29" t="s">
@@ -6760,15 +6765,15 @@
       </c>
       <c r="I156" s="31"/>
     </row>
-    <row r="157" spans="1:9" ht="30">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="29" t="s">
         <v>180</v>
       </c>
       <c r="B157" s="30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C157" s="31" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D157" s="29"/>
       <c r="E157" s="29" t="s">
@@ -6785,7 +6790,7 @@
       </c>
       <c r="I157" s="31"/>
     </row>
-    <row r="158" spans="1:9" ht="45">
+    <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="29" t="s">
         <v>181</v>
       </c>
@@ -6793,7 +6798,7 @@
         <v>32</v>
       </c>
       <c r="C158" s="31" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D158" s="29"/>
       <c r="E158" s="29" t="s">
@@ -6810,7 +6815,7 @@
       </c>
       <c r="I158" s="31"/>
     </row>
-    <row r="159" spans="1:9" ht="45">
+    <row r="159" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="29" t="s">
         <v>182</v>
       </c>
@@ -6818,7 +6823,7 @@
         <v>32</v>
       </c>
       <c r="C159" s="31" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D159" s="29"/>
       <c r="E159" s="29" t="s">
@@ -6835,7 +6840,7 @@
       </c>
       <c r="I159" s="31"/>
     </row>
-    <row r="160" spans="1:9" ht="30">
+    <row r="160" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="29" t="s">
         <v>183</v>
       </c>
@@ -6843,7 +6848,7 @@
         <v>32</v>
       </c>
       <c r="C160" s="31" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D160" s="29"/>
       <c r="E160" s="29" t="s">
@@ -6860,7 +6865,7 @@
       </c>
       <c r="I160" s="31"/>
     </row>
-    <row r="161" spans="1:9" ht="60">
+    <row r="161" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A161" s="29" t="s">
         <v>184</v>
       </c>
@@ -6868,7 +6873,7 @@
         <v>32</v>
       </c>
       <c r="C161" s="31" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D161" s="29"/>
       <c r="E161" s="29" t="s">
@@ -6885,7 +6890,7 @@
       </c>
       <c r="I161" s="31"/>
     </row>
-    <row r="162" spans="1:9" ht="60">
+    <row r="162" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="29" t="s">
         <v>185</v>
       </c>
@@ -6893,7 +6898,7 @@
         <v>32</v>
       </c>
       <c r="C162" s="31" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D162" s="29"/>
       <c r="E162" s="29" t="s">
@@ -6910,7 +6915,7 @@
       </c>
       <c r="I162" s="31"/>
     </row>
-    <row r="163" spans="1:9" ht="30">
+    <row r="163" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="29" t="s">
         <v>186</v>
       </c>
@@ -6918,7 +6923,7 @@
         <v>32</v>
       </c>
       <c r="C163" s="31" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D163" s="29"/>
       <c r="E163" s="29" t="s">
@@ -6935,7 +6940,7 @@
       </c>
       <c r="I163" s="31"/>
     </row>
-    <row r="164" spans="1:9" ht="45">
+    <row r="164" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="29" t="s">
         <v>187</v>
       </c>
@@ -6943,7 +6948,7 @@
         <v>32</v>
       </c>
       <c r="C164" s="31" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D164" s="29"/>
       <c r="E164" s="29" t="s">
@@ -6960,7 +6965,7 @@
       </c>
       <c r="I164" s="31"/>
     </row>
-    <row r="165" spans="1:9" ht="45">
+    <row r="165" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="29" t="s">
         <v>188</v>
       </c>
@@ -6968,7 +6973,7 @@
         <v>32</v>
       </c>
       <c r="C165" s="31" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="29" t="s">
@@ -6985,7 +6990,7 @@
       </c>
       <c r="I165" s="31"/>
     </row>
-    <row r="166" spans="1:9" ht="30">
+    <row r="166" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="29" t="s">
         <v>189</v>
       </c>
@@ -6993,7 +6998,7 @@
         <v>32</v>
       </c>
       <c r="C166" s="31" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D166" s="29"/>
       <c r="E166" s="29" t="s">
@@ -7010,7 +7015,7 @@
       </c>
       <c r="I166" s="31"/>
     </row>
-    <row r="167" spans="1:9" ht="45">
+    <row r="167" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="29" t="s">
         <v>190</v>
       </c>
@@ -7018,7 +7023,7 @@
         <v>32</v>
       </c>
       <c r="C167" s="31" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D167" s="29"/>
       <c r="E167" s="29" t="s">
@@ -7035,7 +7040,7 @@
       </c>
       <c r="I167" s="31"/>
     </row>
-    <row r="168" spans="1:9" ht="30">
+    <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="29" t="s">
         <v>191</v>
       </c>
@@ -7043,7 +7048,7 @@
         <v>32</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D168" s="29"/>
       <c r="E168" s="29" t="s">
@@ -7060,7 +7065,7 @@
       </c>
       <c r="I168" s="31"/>
     </row>
-    <row r="169" spans="1:9" ht="45">
+    <row r="169" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="29" t="s">
         <v>192</v>
       </c>
@@ -7068,7 +7073,7 @@
         <v>32</v>
       </c>
       <c r="C169" s="31" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D169" s="29"/>
       <c r="E169" s="29" t="s">
@@ -7085,7 +7090,7 @@
       </c>
       <c r="I169" s="31"/>
     </row>
-    <row r="170" spans="1:9" ht="45">
+    <row r="170" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="29" t="s">
         <v>193</v>
       </c>
@@ -7093,7 +7098,7 @@
         <v>33</v>
       </c>
       <c r="C170" s="31" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D170" s="29"/>
       <c r="E170" s="29" t="s">
@@ -7110,7 +7115,7 @@
       </c>
       <c r="I170" s="31"/>
     </row>
-    <row r="171" spans="1:9" ht="45">
+    <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="29" t="s">
         <v>194</v>
       </c>
@@ -7118,7 +7123,7 @@
         <v>33</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D171" s="29"/>
       <c r="E171" s="29" t="s">
@@ -7135,7 +7140,7 @@
       </c>
       <c r="I171" s="31"/>
     </row>
-    <row r="172" spans="1:9" ht="30">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="29" t="s">
         <v>195</v>
       </c>
@@ -7143,7 +7148,7 @@
         <v>33</v>
       </c>
       <c r="C172" s="31" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D172" s="29"/>
       <c r="E172" s="29" t="s">
@@ -7160,7 +7165,7 @@
       </c>
       <c r="I172" s="31"/>
     </row>
-    <row r="173" spans="1:9" ht="45">
+    <row r="173" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="29" t="s">
         <v>196</v>
       </c>
@@ -7168,7 +7173,7 @@
         <v>33</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="29" t="s">
@@ -7185,7 +7190,7 @@
       </c>
       <c r="I173" s="31"/>
     </row>
-    <row r="174" spans="1:9" ht="60">
+    <row r="174" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" s="29" t="s">
         <v>197</v>
       </c>
@@ -7193,7 +7198,7 @@
         <v>33</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D174" s="29"/>
       <c r="E174" s="29" t="s">
@@ -7210,15 +7215,15 @@
       </c>
       <c r="I174" s="31"/>
     </row>
-    <row r="175" spans="1:9" ht="60">
+    <row r="175" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A175" s="29" t="s">
         <v>198</v>
       </c>
       <c r="B175" s="30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="29" t="s">
@@ -7235,15 +7240,15 @@
       </c>
       <c r="I175" s="31"/>
     </row>
-    <row r="176" spans="1:9" ht="45">
+    <row r="176" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="29" t="s">
         <v>199</v>
       </c>
       <c r="B176" s="30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D176" s="29"/>
       <c r="E176" s="29" t="s">
@@ -7260,15 +7265,15 @@
       </c>
       <c r="I176" s="31"/>
     </row>
-    <row r="177" spans="1:9" ht="45">
+    <row r="177" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="29" t="s">
         <v>200</v>
       </c>
       <c r="B177" s="30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C177" s="31" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D177" s="29"/>
       <c r="E177" s="29" t="s">
@@ -7285,15 +7290,15 @@
       </c>
       <c r="I177" s="31"/>
     </row>
-    <row r="178" spans="1:9" ht="30">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="29" t="s">
         <v>201</v>
       </c>
       <c r="B178" s="30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D178" s="29"/>
       <c r="E178" s="29" t="s">
@@ -7310,15 +7315,15 @@
       </c>
       <c r="I178" s="31"/>
     </row>
-    <row r="179" spans="1:9" ht="60">
+    <row r="179" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="29" t="s">
         <v>202</v>
       </c>
       <c r="B179" s="30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D179" s="29"/>
       <c r="E179" s="29" t="s">
@@ -7335,15 +7340,15 @@
       </c>
       <c r="I179" s="31"/>
     </row>
-    <row r="180" spans="1:9" ht="45">
+    <row r="180" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="29" t="s">
         <v>203</v>
       </c>
       <c r="B180" s="30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D180" s="29"/>
       <c r="E180" s="29" t="s">
@@ -7360,15 +7365,15 @@
       </c>
       <c r="I180" s="31"/>
     </row>
-    <row r="181" spans="1:9" ht="30">
+    <row r="181" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" s="29" t="s">
         <v>204</v>
       </c>
       <c r="B181" s="30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D181" s="29"/>
       <c r="E181" s="29" t="s">
@@ -7385,15 +7390,15 @@
       </c>
       <c r="I181" s="31"/>
     </row>
-    <row r="182" spans="1:9" ht="60">
+    <row r="182" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="29" t="s">
         <v>205</v>
       </c>
       <c r="B182" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D182" s="29"/>
       <c r="E182" s="29" t="s">
@@ -7410,15 +7415,15 @@
       </c>
       <c r="I182" s="31"/>
     </row>
-    <row r="183" spans="1:9" ht="60">
+    <row r="183" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="29" t="s">
         <v>206</v>
       </c>
       <c r="B183" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C183" s="31" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D183" s="29"/>
       <c r="E183" s="29" t="s">
@@ -7435,15 +7440,15 @@
       </c>
       <c r="I183" s="31"/>
     </row>
-    <row r="184" spans="1:9" ht="60">
+    <row r="184" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="29" t="s">
         <v>207</v>
       </c>
       <c r="B184" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="29" t="s">
@@ -7460,15 +7465,15 @@
       </c>
       <c r="I184" s="31"/>
     </row>
-    <row r="185" spans="1:9" ht="45">
+    <row r="185" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" s="29" t="s">
         <v>208</v>
       </c>
       <c r="B185" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C185" s="31" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D185" s="29"/>
       <c r="E185" s="29" t="s">
@@ -7485,15 +7490,15 @@
       </c>
       <c r="I185" s="31"/>
     </row>
-    <row r="186" spans="1:9" ht="45">
+    <row r="186" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="29" t="s">
         <v>209</v>
       </c>
       <c r="B186" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C186" s="31" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="29" t="s">
@@ -7510,15 +7515,15 @@
       </c>
       <c r="I186" s="31"/>
     </row>
-    <row r="187" spans="1:9" ht="30">
+    <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="29" t="s">
         <v>210</v>
       </c>
       <c r="B187" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="29" t="s">
@@ -7535,15 +7540,15 @@
       </c>
       <c r="I187" s="31"/>
     </row>
-    <row r="188" spans="1:9" ht="30">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="29" t="s">
         <v>211</v>
       </c>
       <c r="B188" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="29" t="s">
@@ -7560,15 +7565,15 @@
       </c>
       <c r="I188" s="31"/>
     </row>
-    <row r="189" spans="1:9" ht="45">
+    <row r="189" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" s="29" t="s">
         <v>212</v>
       </c>
       <c r="B189" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D189" s="29"/>
       <c r="E189" s="29" t="s">
@@ -7585,15 +7590,15 @@
       </c>
       <c r="I189" s="31"/>
     </row>
-    <row r="190" spans="1:9" ht="30">
+    <row r="190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="29" t="s">
         <v>213</v>
       </c>
       <c r="B190" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D190" s="29"/>
       <c r="E190" s="29" t="s">
@@ -7610,15 +7615,15 @@
       </c>
       <c r="I190" s="31"/>
     </row>
-    <row r="191" spans="1:9" ht="45">
+    <row r="191" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="29" t="s">
         <v>214</v>
       </c>
       <c r="B191" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D191" s="29"/>
       <c r="E191" s="29" t="s">
@@ -7635,15 +7640,15 @@
       </c>
       <c r="I191" s="31"/>
     </row>
-    <row r="192" spans="1:9" ht="45">
+    <row r="192" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="29" t="s">
         <v>215</v>
       </c>
       <c r="B192" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D192" s="29"/>
       <c r="E192" s="29" t="s">
@@ -7660,15 +7665,15 @@
       </c>
       <c r="I192" s="31"/>
     </row>
-    <row r="193" spans="1:9" ht="45">
+    <row r="193" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="29" t="s">
         <v>216</v>
       </c>
       <c r="B193" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D193" s="29"/>
       <c r="E193" s="29" t="s">
@@ -7685,15 +7690,15 @@
       </c>
       <c r="I193" s="31"/>
     </row>
-    <row r="194" spans="1:9" ht="45">
+    <row r="194" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="29" t="s">
         <v>217</v>
       </c>
       <c r="B194" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D194" s="29"/>
       <c r="E194" s="29" t="s">
@@ -7710,15 +7715,15 @@
       </c>
       <c r="I194" s="31"/>
     </row>
-    <row r="195" spans="1:9" ht="45">
+    <row r="195" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A195" s="29" t="s">
         <v>218</v>
       </c>
       <c r="B195" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D195" s="29"/>
       <c r="E195" s="29" t="s">
@@ -7735,15 +7740,15 @@
       </c>
       <c r="I195" s="31"/>
     </row>
-    <row r="196" spans="1:9" ht="45">
+    <row r="196" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="29" t="s">
         <v>219</v>
       </c>
       <c r="B196" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -7760,15 +7765,15 @@
       </c>
       <c r="I196" s="31"/>
     </row>
-    <row r="197" spans="1:9" ht="45">
+    <row r="197" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A197" s="29" t="s">
         <v>220</v>
       </c>
       <c r="B197" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C197" s="31" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D197" s="29"/>
       <c r="E197" s="29" t="s">
@@ -7785,15 +7790,15 @@
       </c>
       <c r="I197" s="31"/>
     </row>
-    <row r="198" spans="1:9" ht="30">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="29" t="s">
         <v>221</v>
       </c>
       <c r="B198" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C198" s="31" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -7810,15 +7815,15 @@
       </c>
       <c r="I198" s="31"/>
     </row>
-    <row r="199" spans="1:9" ht="45">
+    <row r="199" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A199" s="29" t="s">
         <v>222</v>
       </c>
       <c r="B199" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C199" s="31" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D199" s="29"/>
       <c r="E199" s="29" t="s">
@@ -7835,15 +7840,15 @@
       </c>
       <c r="I199" s="31"/>
     </row>
-    <row r="200" spans="1:9" ht="45">
+    <row r="200" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A200" s="29" t="s">
         <v>223</v>
       </c>
       <c r="B200" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D200" s="29"/>
       <c r="E200" s="29" t="s">
@@ -7860,15 +7865,15 @@
       </c>
       <c r="I200" s="31"/>
     </row>
-    <row r="201" spans="1:9" ht="45">
+    <row r="201" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="29" t="s">
         <v>224</v>
       </c>
       <c r="B201" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C201" s="31" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -7885,15 +7890,15 @@
       </c>
       <c r="I201" s="31"/>
     </row>
-    <row r="202" spans="1:9" ht="60">
+    <row r="202" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A202" s="29" t="s">
         <v>225</v>
       </c>
       <c r="B202" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C202" s="31" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D202" s="29"/>
       <c r="E202" s="29" t="s">
@@ -7910,15 +7915,15 @@
       </c>
       <c r="I202" s="31"/>
     </row>
-    <row r="203" spans="1:9" ht="45">
+    <row r="203" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" s="29" t="s">
         <v>226</v>
       </c>
       <c r="B203" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C203" s="31" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D203" s="29"/>
       <c r="E203" s="29" t="s">
@@ -7935,15 +7940,15 @@
       </c>
       <c r="I203" s="31"/>
     </row>
-    <row r="204" spans="1:9" ht="75">
+    <row r="204" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A204" s="29" t="s">
         <v>227</v>
       </c>
       <c r="B204" s="30" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C204" s="31" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D204" s="29"/>
       <c r="E204" s="29" t="s">
@@ -7960,15 +7965,15 @@
       </c>
       <c r="I204" s="31"/>
     </row>
-    <row r="205" spans="1:9" ht="45">
+    <row r="205" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A205" s="29" t="s">
         <v>228</v>
       </c>
       <c r="B205" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C205" s="31" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D205" s="29"/>
       <c r="E205" s="29" t="s">
@@ -7985,15 +7990,15 @@
       </c>
       <c r="I205" s="31"/>
     </row>
-    <row r="206" spans="1:9" ht="30">
+    <row r="206" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="29" t="s">
         <v>229</v>
       </c>
       <c r="B206" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C206" s="31" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D206" s="29"/>
       <c r="E206" s="29" t="s">
@@ -8010,15 +8015,15 @@
       </c>
       <c r="I206" s="31"/>
     </row>
-    <row r="207" spans="1:9" ht="45">
+    <row r="207" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="29" t="s">
         <v>230</v>
       </c>
       <c r="B207" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C207" s="31" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D207" s="29"/>
       <c r="E207" s="29" t="s">
@@ -8035,15 +8040,15 @@
       </c>
       <c r="I207" s="31"/>
     </row>
-    <row r="208" spans="1:9" ht="45">
-      <c r="A208" s="29" t="s">
-        <v>231</v>
+    <row r="208" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A208" s="22" t="s">
+        <v>505</v>
       </c>
       <c r="B208" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C208" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D208" s="29"/>
       <c r="E208" s="29" t="s">
@@ -8060,18 +8065,18 @@
       </c>
       <c r="I208" s="31"/>
     </row>
-    <row r="209" spans="1:9" ht="45">
+    <row r="209" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A209" s="22" t="s">
+        <v>484</v>
+      </c>
+      <c r="B209" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="C209" s="31" t="s">
         <v>486</v>
       </c>
-      <c r="B209" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="C209" s="31" t="s">
-        <v>488</v>
-      </c>
       <c r="D209" s="29" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E209" s="29" t="s">
         <v>22</v>
@@ -8087,18 +8092,18 @@
       </c>
       <c r="I209" s="31"/>
     </row>
-    <row r="210" spans="1:9" ht="45">
+    <row r="210" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A210" s="29" t="s">
+        <v>485</v>
+      </c>
+      <c r="B210" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="C210" s="31" t="s">
         <v>487</v>
       </c>
-      <c r="B210" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="C210" s="31" t="s">
-        <v>489</v>
-      </c>
       <c r="D210" s="29" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E210" s="29" t="s">
         <v>22</v>
@@ -8113,21 +8118,21 @@
         <v>20</v>
       </c>
       <c r="I210" s="31" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9" ht="45">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" s="29" t="s">
+        <v>490</v>
+      </c>
+      <c r="B211" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="C211" s="31" t="s">
+        <v>489</v>
+      </c>
+      <c r="D211" s="29" t="s">
         <v>492</v>
-      </c>
-      <c r="B211" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="C211" s="31" t="s">
-        <v>491</v>
-      </c>
-      <c r="D211" s="29" t="s">
-        <v>494</v>
       </c>
       <c r="E211" s="29" t="s">
         <v>22</v>
@@ -8142,21 +8147,21 @@
         <v>20</v>
       </c>
       <c r="I211" s="31" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="212" spans="1:9" ht="60">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A212" s="29" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B212" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C212" s="31" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E212" s="29" t="s">
         <v>22</v>
@@ -8171,15 +8176,15 @@
         <v>20</v>
       </c>
       <c r="I212" s="31" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="213" spans="1:9" ht="105">
-      <c r="A213" s="29" t="s">
-        <v>232</v>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A213" s="22" t="s">
+        <v>507</v>
       </c>
       <c r="B213" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C213" s="20" t="s">
         <v>506</v>
@@ -8199,15 +8204,15 @@
       </c>
       <c r="I213" s="31"/>
     </row>
-    <row r="214" spans="1:9" ht="45">
+    <row r="214" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A214" s="29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B214" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C214" s="31" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D214" s="29"/>
       <c r="E214" s="29" t="s">
@@ -8224,15 +8229,15 @@
       </c>
       <c r="I214" s="31"/>
     </row>
-    <row r="215" spans="1:9" ht="45">
+    <row r="215" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A215" s="29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B215" s="30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C215" s="31" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D215" s="29"/>
       <c r="E215" s="29" t="s">
@@ -8248,18 +8253,18 @@
         <v>21</v>
       </c>
       <c r="I215" s="31" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="216" spans="1:9">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B216" s="30" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C216" s="31" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D216" s="29"/>
       <c r="E216" s="29" t="s">
@@ -8276,15 +8281,15 @@
       </c>
       <c r="I216" s="31"/>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="29" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B217" s="30" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C217" s="31" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D217" s="29"/>
       <c r="E217" s="29" t="s">
@@ -8301,15 +8306,15 @@
       </c>
       <c r="I217" s="31"/>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="29" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B218" s="30" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C218" s="31" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D218" s="29"/>
       <c r="E218" s="29" t="s">
@@ -8326,15 +8331,15 @@
       </c>
       <c r="I218" s="31"/>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="29" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B219" s="30" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C219" s="31" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D219" s="29"/>
       <c r="E219" s="29" t="s">
@@ -8351,15 +8356,15 @@
       </c>
       <c r="I219" s="31"/>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="29" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B220" s="30" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C220" s="31" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D220" s="29"/>
       <c r="E220" s="29" t="s">
@@ -8376,15 +8381,15 @@
       </c>
       <c r="I220" s="31"/>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="29" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B221" s="30" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C221" s="31" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D221" s="29"/>
       <c r="E221" s="29" t="s">
@@ -8401,15 +8406,15 @@
       </c>
       <c r="I221" s="31"/>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="29" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B222" s="30" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C222" s="31" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D222" s="29"/>
       <c r="E222" s="29" t="s">
@@ -8426,15 +8431,15 @@
       </c>
       <c r="I222" s="31"/>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="29" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B223" s="30" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C223" s="31" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D223" s="29"/>
       <c r="E223" s="29" t="s">
@@ -8451,15 +8456,15 @@
       </c>
       <c r="I223" s="31"/>
     </row>
-    <row r="224" spans="1:9" ht="45">
+    <row r="224" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A224" s="29" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B224" s="30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C224" s="31" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D224" s="29"/>
       <c r="E224" s="29" t="s">
@@ -8476,15 +8481,15 @@
       </c>
       <c r="I224" s="31"/>
     </row>
-    <row r="225" spans="1:9" ht="30">
+    <row r="225" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="29" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B225" s="30" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C225" s="31" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D225" s="29"/>
       <c r="E225" s="29" t="s">
@@ -8501,15 +8506,15 @@
       </c>
       <c r="I225" s="31"/>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="29" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B226" s="30" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C226" s="31" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D226" s="29"/>
       <c r="E226" s="29" t="s">
@@ -8526,15 +8531,15 @@
       </c>
       <c r="I226" s="31"/>
     </row>
-    <row r="227" spans="1:9" ht="30">
+    <row r="227" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="29" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B227" s="30" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C227" s="31" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D227" s="29"/>
       <c r="E227" s="29" t="s">
@@ -8551,15 +8556,15 @@
       </c>
       <c r="I227" s="31"/>
     </row>
-    <row r="228" spans="1:9" ht="30">
+    <row r="228" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B228" s="30" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C228" s="31" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D228" s="29"/>
       <c r="E228" s="29" t="s">
@@ -8576,15 +8581,15 @@
       </c>
       <c r="I228" s="31"/>
     </row>
-    <row r="229" spans="1:9" ht="45">
+    <row r="229" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="29" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B229" s="30" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C229" s="31" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D229" s="29"/>
       <c r="E229" s="29" t="s">
@@ -8601,15 +8606,15 @@
       </c>
       <c r="I229" s="31"/>
     </row>
-    <row r="230" spans="1:9" ht="30">
+    <row r="230" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="29" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B230" s="30" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C230" s="31" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D230" s="29"/>
       <c r="E230" s="29" t="s">
@@ -8626,15 +8631,15 @@
       </c>
       <c r="I230" s="31"/>
     </row>
-    <row r="231" spans="1:9" ht="30">
+    <row r="231" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="29" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B231" s="30" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C231" s="31" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D231" s="29"/>
       <c r="E231" s="29" t="s">
@@ -8651,11 +8656,11 @@
       </c>
       <c r="I231" s="31"/>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="3"/>
       <c r="B232" s="10"/>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="3"/>
       <c r="B233" s="10"/>
     </row>
@@ -8761,12 +8766,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -8815,7 +8814,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8824,21 +8823,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8853,10 +8844,24 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>